<commit_message>
Added updated changelog for v1.02
</commit_message>
<xml_diff>
--- a/CDR Test Documentation CHANGE LOG.xlsx
+++ b/CDR Test Documentation CHANGE LOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://govteams.sharepoint.com/sites/datastandardsbody/Shared Documents/Standards and Guidelines/Testing/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codeRepos\codeDataStandards\standards-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{9B3D86EA-31BB-4D21-B7B8-766CEFF32DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E963F3A-452E-408A-BFC9-9C219B075334}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{432D017D-E142-4B8A-8A0F-A5AFD8FC20C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1E61262-89E5-4C9F-B6BD-CA910CFEB013}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{E1E61262-89E5-4C9F-B6BD-CA910CFEB013}"/>
   </bookViews>
   <sheets>
     <sheet name="Change log" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="229">
   <si>
     <t>Change date</t>
   </si>
@@ -386,13 +386,538 @@
   </si>
   <si>
     <t xml:space="preserve">A.CFC.001 added  </t>
+  </si>
+  <si>
+    <t>T.EAR.001</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>T.EAR.033</t>
+  </si>
+  <si>
+    <t>T.EAR.109</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added link to Postman examples </t>
+  </si>
+  <si>
+    <t>1.0.2</t>
+  </si>
+  <si>
+    <t>A.EAR.001</t>
+  </si>
+  <si>
+    <t>A.EAR.002</t>
+  </si>
+  <si>
+    <t>A.EAR.003</t>
+  </si>
+  <si>
+    <t>A.EAR.004</t>
+  </si>
+  <si>
+    <t>A.EAR.005</t>
+  </si>
+  <si>
+    <t>A.EAR.006</t>
+  </si>
+  <si>
+    <t>A.EAR.007</t>
+  </si>
+  <si>
+    <t>A.EAR.008</t>
+  </si>
+  <si>
+    <t>A.EAR.009</t>
+  </si>
+  <si>
+    <t>A.EAR.010</t>
+  </si>
+  <si>
+    <t>A.EAR.011</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given; When </t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the ADR to DH request 
+to 
+the {servicePointId} is included AND the {servicePointId} value is valid 
+Changed the {servicePointId} value is valid 
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the ADR to DH request url
+to
+the {servicePointId} is included AND the requested service point is permanently unavailable. (No subsequent request for the service point will be successful.)
+Changed The requested service point is permanently unavailable. (No subsequent request for the service point will be successful.) 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When </t>
+  </si>
+  <si>
+    <t>Changed the DH receives the request AND interprets the Body
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted by the ADR
+Changed the DH receives the request 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>A.EAS.001</t>
+  </si>
+  <si>
+    <t>A.EAS.002</t>
+  </si>
+  <si>
+    <t>A.EAS.003</t>
+  </si>
+  <si>
+    <t>A.EAS.004</t>
+  </si>
+  <si>
+    <t>A.EAS.005</t>
+  </si>
+  <si>
+    <t>A.EAS.006</t>
+  </si>
+  <si>
+    <t>A.EAS.007</t>
+  </si>
+  <si>
+    <t>A.EAS.008</t>
+  </si>
+  <si>
+    <t>A.EAS.009</t>
+  </si>
+  <si>
+    <t>A.EAS.010</t>
+  </si>
+  <si>
+    <t>A.EAS.011</t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the DH to SDH request 
+to 
+the {servicePointId} is included AND the {servicePointId} value is valid 
+Changed the {servicePointId} value is valid 
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the DH to SDH request 
+to
+the {servicePointId} is included AND the requested service point is permanently unavailable. (No subsequent request for the service point will be successful.)
+Changed The requested service point is permanently unavailable. (No subsequent request for the service point will be successful.) 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the ADR to DH request url
+to
+the {servicePointId} is included AND the requested service point is temporarily unavailable. (Subsequent requests for the service point may be successful.)
+Changed The requested service point is temporarily unavailable. (Subsequent requests for the service point may be successful.) 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the {servicePointId} is included in the DH to SDH request 
+to
+the {servicePointId} is included AND the requested service point is temporarily unavailable. (Subsequent requests for the service point may be successful.)
+Changed The requested service point is temporarily unavailable.  (Subsequent requests for the service point may be successful.)
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted by the ADR 
+Changed the DH receives the request
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted by the DH 
+Changed the SDH receives the request
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in the DH to SDH request 
+Changed the {servicePointId} value is valid AND the request is formated correctly
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the SDH receives the request and interprets the Body
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in the ADR to DH request AND added AND the {servicePointId} value is valid 
+Changed the {servicePointId} value is valid 
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in the ADR to DH request AND added AND the {servicePointId} value is valid AND the request is formated correctly
+Changed the {servicePointId} value is valid AND the request is formated correctly
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the {servicePointId} value is valid 
+Changed the {servicePointId} value is valid 
+to 
+response is returned</t>
+  </si>
+  <si>
+    <t>When</t>
+  </si>
+  <si>
+    <t>Changed the SDH receives the request and interprets the Body
+to
+response is returned</t>
+  </si>
+  <si>
+    <t>A.CPG.001</t>
+  </si>
+  <si>
+    <t>A.CPG.002</t>
+  </si>
+  <si>
+    <t>A.CPG.003</t>
+  </si>
+  <si>
+    <t>A.CPG.004</t>
+  </si>
+  <si>
+    <t>A.CPG.005</t>
+  </si>
+  <si>
+    <t>A.CVN.001</t>
+  </si>
+  <si>
+    <t>A.CVN.002</t>
+  </si>
+  <si>
+    <t>A.CVN.003</t>
+  </si>
+  <si>
+    <t>A.CFI.001</t>
+  </si>
+  <si>
+    <t>A.CFI.003</t>
+  </si>
+  <si>
+    <t>A.CFA.001</t>
+  </si>
+  <si>
+    <t>A.CFA.002</t>
+  </si>
+  <si>
+    <t>A.CFA.003</t>
+  </si>
+  <si>
+    <t>A.CFA.004</t>
+  </si>
+  <si>
+    <t>A.CFC.001</t>
+  </si>
+  <si>
+    <t>A.CFC.002</t>
+  </si>
+  <si>
+    <t>A.CFC.003</t>
+  </si>
+  <si>
+    <t>A.CCH.001</t>
+  </si>
+  <si>
+    <t>A.CCH.002</t>
+  </si>
+  <si>
+    <t>A.CCH.003</t>
+  </si>
+  <si>
+    <t>A.CAI.001</t>
+  </si>
+  <si>
+    <t>A.CAI.002</t>
+  </si>
+  <si>
+    <t>A.CAI.003</t>
+  </si>
+  <si>
+    <t>A.COD.001</t>
+  </si>
+  <si>
+    <t>A.COD.002</t>
+  </si>
+  <si>
+    <t>A.CND.001</t>
+  </si>
+  <si>
+    <t>A.CND.002</t>
+  </si>
+  <si>
+    <t>A.CBD.001</t>
+  </si>
+  <si>
+    <t>Given; When; Then</t>
+  </si>
+  <si>
+    <t>Deleted in a GET Request AND Added AND the page value is a number and page-size is [1,25,1000,null]
+Changed to the page value is a number and page-size is [1,25,1000,null]
+to 
+a response is returned
+AND the response has a status of 200
+Deleted AND the response has a status of 200</t>
+  </si>
+  <si>
+    <t>Deleted in a GET Request AND Added the the value for &lt;page-size&gt; is outside the range [1..1000]
+OR the &lt;page-size&gt; is a not a positive integer
+Changed the value for &lt;page-size&gt; is outside the range [1..1000]
+OR the &lt;page-size&gt; is a not a positive integer
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the &lt;page&gt; is a not a positive integer
+Changed the &lt;page&gt; is a not a positive integer
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the &lt;page&gt; value is greater than the number of pages available 
+Changed the &lt;page&gt; value is greater than the number of pages available 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the page size parameter value is not a positive integer (number)
+Changed the page size parameter value is not a positive integer (number)
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the value for the &lt;x-v&gt; is a positive integer
+Changed the value for the &lt;x-v&gt; is a positive integer
+to 
+a response is returned AND the response has a status of 200
+Deleted the response has a status of 200</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Given; When; Then </t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the version value is not a valid number is [-1,0,1001]
+Changed the version value is not a valid number is [-1,0,1001]
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a GET request AND added AND the verison value is not a valid number is an alpha (e.g. "foo")
+Changed the verison value is not a valid number is an alpha (e.g. "foo")
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the request version &lt;x-v&gt; is not supported
+Changed the request version &lt;x-v&gt; is not supported
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND no version between &lt;x-v&gt; and &lt;x-min-v&gt; is supported
+Changed no version between &lt;x-v&gt; and &lt;x-min-v&gt; is supported
+to  
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted in a get request AND added the value for the &lt;x-min-v&gt;  is a positive integer
+Changed the value for the &lt;x-min-v&gt;  is a positive integer
+to
+a response is returned AND the response has a status of 200</t>
+  </si>
+  <si>
+    <t>Deleted in a get request AND Added AND the &lt;x-min-v&gt; is a not a positive integer
+Changed the &lt;x-min-v&gt; is a not a positive integer
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>ASSERTIONS</t>
+  </si>
+  <si>
+    <t>Added AND the &lt;x-fapi-interaction-id&gt; is in a valid format 
+Changed the &lt;x-fapi-interaction-id&gt; is in a valid format 
+to 
+A response is returned
+Deleted AND</t>
+  </si>
+  <si>
+    <t>Deleted in the GET request AND Added AND the &lt;x-fapi-interaction-id&gt; is not in a valid format 
+Changed the &lt;x-fapi-interaction-id&gt; is not in a valid format 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Changed the called API is a resource call and does require authentication
+to 
+the API requires authentication
+Changed the &lt;x-fapi-auth-date&gt; is present in the request header
+AND is in a valid format
+to 
+a response is returned 
+AND the response has a status of 200
+Changed the response has a status of 200 
+to
+&lt;x-fapi-auth-date&gt; is present in the request header
+AND is in a valid format</t>
+  </si>
+  <si>
+    <t>Changed the called API is a resource call and does require authentication
+to 
+the API requires authentication AND the &lt;x-fapi-auth-date&gt; is NOT present  in the request header
+Changed the &lt;x-fapi-auth-date&gt; is NOT present  in the request header
+to 
+a response is returned 
+Added AND the response body has ErrorListReponse object</t>
+  </si>
+  <si>
+    <t>Changed the called API is a resource call and does require authentication
+to 
+the API requires authentication AND the &lt;x-fapi-auth-date&gt; is in the request header AND is NOT in a valid format
+Changed the &lt;x-fapi-auth-date&gt; is  in the request header
+AND is NOT in a valid format
+to
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added the API requires authentication AND
+Added AND the response has a status of 200</t>
+  </si>
+  <si>
+    <t>Deleted called
+Changed the &lt;x-fapi-customer-ip-address&gt; is present in the request header AND is in a valid IPv4 or IPv6 format
+to 
+a response is returned
+AND the response has a status of 200
+Changed the response has a status of 200
+to 
+the &lt;x-fapi-customer-ip-address&gt; is present in the request header
+AND is in a valid IPv4 or IPv6 format</t>
+  </si>
+  <si>
+    <t>Deleted called AND Added AND the &lt;x-fapi-customer-ip-address&gt; is NOT present in the request header
+Changed the &lt;x-fapi-customer-ip-address&gt; is NOT present in the request header
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted called AND Added AND "the &lt;x-fapi-customer-ip-address&gt; is in present the request header
+AND is NEITHER in a valid IPv4 or IPv6 format"
+Changed AND the &lt;x-fapi-customer-ip-address&gt; in present the request header AND is NEITHER  in a valid IPv4 or IPv6 format
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Deleted called
+Changed the &lt;x-cds-client-headers&gt; is present in the request header AND is Base64 encoded
+to 
+a response is returned AND the response has a status of 200
+Changed the response has a status of 200 
+to 
+the &lt;x-cds-client-headers&gt; is present in the request header AND is Base64 encoded</t>
+  </si>
+  <si>
+    <t>Changed the called API requires authentication AND the call is an attended, ie customer present, call
+to 
+the API requires authentication AND the &lt;x-cds-client-headers&gt; is mandatory AND the &lt;x-cds-client-headers&gt; is NOT present in the request header
+Changed the &lt;x-cds-client-headers&gt; is NOT present in the request header
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed the called API requires authentication AND the call is an attended, ie customer present, call
+to 
+the &lt;x-cds-client-headers&gt;  present the request header AND is Not Base64 encoded
+Changed the &lt;x-cds-client-headers&gt;  present the request header
+AND is Not Base64 encoded 
+to 
+a response is returned </t>
+  </si>
+  <si>
+    <t xml:space="preserve">When; Then </t>
+  </si>
+  <si>
+    <t>Changed the &lt;x-cds-arrangement&gt; is present in the request header AND is in a valid format
+to 
+a response is returned AND the response has a status of 200
+Changed the response has a status of 200
+to 
+the &lt;x-cds-arrangement&gt; is present in the request header AND is in a valid format</t>
+  </si>
+  <si>
+    <t>Added the &lt;x-cds-arrangement&gt; is NOT present in the request header
+Changed the &lt;x-cds-arrangement&gt; is NOT present in the request header
+to  
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the &lt;oldest-date&gt; is in a valid DateString format
+Changed the &lt;oldest-date&gt; is in a valid DateString format
+to  
+a response is returned AND the response has a status of 200
+Deleted AND the response has a status of 200</t>
+  </si>
+  <si>
+    <t>Added the &lt;x-cds-arrangement&gt; is present in the request header AND is NOT in a valid format
+Changed the &lt;x-cds-arrangement&gt; is present in the request header AND is NOT in a valid format
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the &lt;oldest-date&gt; is not in a DateString valid format
+Changed the &lt;oldest-date&gt; is not in a DateString valid format
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the &lt;newest-date&gt; is in a valid DateString format
+Changed the &lt;newest-date&gt; is in a valid DateString format
+to
+a response is returned AND the response has a status of 200
+Deleted the response has a status of 200 AND</t>
+  </si>
+  <si>
+    <t>Added AND the &lt;newest-date&gt; is not in a valid DateString format
+Changed the &lt;newest-date&gt; is not in a valid DateString format
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Added AND the request body is not in a valid JSON format, ie it is malformed
+Changed the request body is not in a valid JSON format, ie it is malformed 
+to 
+a response is returned</t>
+  </si>
+  <si>
+    <t>Corrected various spellings of Response plus typos on Interaction, Version, i.e., formatted and correctly corrected throughout.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,27 +1334,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4B9470-3BCE-4ABB-997A-921DA99601C0}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection pane="bottomRight" activeCell="M49" sqref="M49"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C102" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="E132" sqref="E132"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1"/>
-    <col min="3" max="3" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="110.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.109375" style="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -849,7 +1374,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="45">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8">
         <v>44700</v>
       </c>
@@ -869,7 +1394,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="8">
         <v>44715</v>
       </c>
@@ -889,7 +1414,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="8">
         <v>44715</v>
       </c>
@@ -909,7 +1434,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="8">
         <v>44715</v>
       </c>
@@ -929,7 +1454,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="8">
         <v>44715</v>
       </c>
@@ -949,7 +1474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="8">
         <v>44715</v>
       </c>
@@ -969,7 +1494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="8">
         <v>44715</v>
       </c>
@@ -989,7 +1514,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="8">
         <v>44715</v>
       </c>
@@ -1009,7 +1534,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="8">
         <v>44715</v>
       </c>
@@ -1029,7 +1554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="8">
         <v>44715</v>
       </c>
@@ -1049,7 +1574,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="8">
         <v>44715</v>
       </c>
@@ -1069,7 +1594,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="8">
         <v>44715</v>
       </c>
@@ -1089,7 +1614,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="8">
         <v>44715</v>
       </c>
@@ -1109,7 +1634,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
         <v>44715</v>
       </c>
@@ -1129,7 +1654,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
         <v>44715</v>
       </c>
@@ -1149,7 +1674,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
         <v>44715</v>
       </c>
@@ -1169,7 +1694,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
         <v>44715</v>
       </c>
@@ -1189,7 +1714,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="8">
         <v>44715</v>
       </c>
@@ -1209,7 +1734,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="8">
         <v>44715</v>
       </c>
@@ -1229,7 +1754,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="8">
         <v>44715</v>
       </c>
@@ -1249,7 +1774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="8">
         <v>44715</v>
       </c>
@@ -1269,7 +1794,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="8">
         <v>44715</v>
       </c>
@@ -1289,7 +1814,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="8">
         <v>44715</v>
       </c>
@@ -1309,7 +1834,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="8">
         <v>44715</v>
       </c>
@@ -1329,7 +1854,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="8">
         <v>44715</v>
       </c>
@@ -1349,7 +1874,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="8">
         <v>44715</v>
       </c>
@@ -1369,7 +1894,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="8">
         <v>44715</v>
       </c>
@@ -1389,7 +1914,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>44715</v>
       </c>
@@ -1409,7 +1934,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="8">
         <v>44715</v>
       </c>
@@ -1429,7 +1954,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="8">
         <v>44715</v>
       </c>
@@ -1449,7 +1974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="8">
         <v>44715</v>
       </c>
@@ -1469,7 +1994,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="8">
         <v>44715</v>
       </c>
@@ -1489,7 +2014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="8">
         <v>44715</v>
       </c>
@@ -1509,7 +2034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="8">
         <v>44715</v>
       </c>
@@ -1529,7 +2054,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="8">
         <v>44715</v>
       </c>
@@ -1549,7 +2074,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="8">
         <v>44715</v>
       </c>
@@ -1569,7 +2094,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="8">
         <v>44715</v>
       </c>
@@ -1589,7 +2114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="8">
         <v>44715</v>
       </c>
@@ -1609,7 +2134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="8">
         <v>44715</v>
       </c>
@@ -1629,7 +2154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="8">
         <v>44715</v>
       </c>
@@ -1649,7 +2174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="8">
         <v>44715</v>
       </c>
@@ -1669,7 +2194,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="8">
         <v>44715</v>
       </c>
@@ -1689,7 +2214,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="8">
         <v>44715</v>
       </c>
@@ -1709,7 +2234,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:6">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="8">
         <v>44715</v>
       </c>
@@ -1729,7 +2254,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="8">
         <v>44715</v>
       </c>
@@ -1749,7 +2274,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:6">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="8">
         <v>44715</v>
       </c>
@@ -1769,7 +2294,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:6">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="8">
         <v>44715</v>
       </c>
@@ -1789,7 +2314,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="8">
         <v>44715</v>
       </c>
@@ -1809,7 +2334,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="8">
         <v>44715</v>
       </c>
@@ -1829,7 +2354,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="8">
         <v>44715</v>
       </c>
@@ -1849,7 +2374,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="8">
         <v>44715</v>
       </c>
@@ -1869,7 +2394,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="8">
         <v>44715</v>
       </c>
@@ -1889,7 +2414,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="8">
         <v>44715</v>
       </c>
@@ -1909,7 +2434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="8">
         <v>44715</v>
       </c>
@@ -1929,7 +2454,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="8">
         <v>44715</v>
       </c>
@@ -1949,7 +2474,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="8">
         <v>44715</v>
       </c>
@@ -1969,7 +2494,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:6">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="8">
         <v>44715</v>
       </c>
@@ -1989,7 +2514,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:6">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="8">
         <v>44715</v>
       </c>
@@ -2009,7 +2534,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:6">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="8">
         <v>44715</v>
       </c>
@@ -2029,7 +2554,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:6">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="8">
         <v>44715</v>
       </c>
@@ -2049,7 +2574,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="30">
+    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="8">
         <v>44715</v>
       </c>
@@ -2069,7 +2594,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:6">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="8">
         <v>44719</v>
       </c>
@@ -2089,7 +2614,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:6">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="8">
         <v>44719</v>
       </c>
@@ -2109,7 +2634,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:6">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="8">
         <v>44719</v>
       </c>
@@ -2129,7 +2654,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:6">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="8">
         <v>44719</v>
       </c>
@@ -2149,7 +2674,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:6">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="8">
         <v>44719</v>
       </c>
@@ -2169,7 +2694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:6">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="8">
         <v>44719</v>
       </c>
@@ -2187,6 +2712,1163 @@
       </c>
       <c r="F68" s="4">
         <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C69" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E69" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F69" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C70" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E70" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F70" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C71" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E71" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F71" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E72" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F72" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E73" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F73" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E74" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F74" s="4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E75" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F75" s="4"/>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E76" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="F76" s="4"/>
+    </row>
+    <row r="77" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A77" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E77" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="F77" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E78" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="F78" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A79" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E79" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="F79" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A80" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="F80" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A81" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="F81" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A82" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E82" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F82" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A83" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E83" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="F83" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A84" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E84" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F84" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A85" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E85" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="F85" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A86" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E86" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F86" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A87" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E87" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F87" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A88" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E88" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="F88" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A89" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E89" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F89" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A90" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B90" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E90" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="F90" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A91" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B91" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="F91" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A92" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E92" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="F92" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A93" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="E93" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="F93" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A94" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E94" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="F94" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A95" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E95" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F95" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A96" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E96" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F96" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A97" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E97" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F97" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A98" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E98" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="F98" s="4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A99" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E99" s="9" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A100" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E100" s="9" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A101" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E101" s="9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A102" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B102" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D102" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E102" s="9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A103" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E103" s="9" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A104" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E104" s="9" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A105" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E105" s="9" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A106" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E106" s="9" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A107" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E107" s="9" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A108" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E108" s="9" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A109" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" s="9" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A110" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E110" s="9" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A111" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E111" s="9" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A112" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B112" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E112" s="9" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A113" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B113" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D113" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E113" s="9" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A114" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B114" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E114" s="9" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A115" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B115" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E115" s="9" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A116" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B116" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E116" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A117" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B117" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E117" s="9" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="118" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A118" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B118" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E118" s="9" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A119" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B119" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E119" s="9" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A120" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B120" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E120" s="9" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="121" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A121" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B121" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E121" s="9" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="122" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A122" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B122" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E122" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A123" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="E123" s="9" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A124" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B124" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E124" s="9" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="125" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A125" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E125" s="9" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A126" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B126" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E126" s="9" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A127" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E127" s="9" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="A128" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="E128" s="9" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A129" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E129" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A130" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E130" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A131" s="8">
+        <v>44754</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -2200,33 +3882,18 @@
     <hyperlink ref="F63" r:id="rId6" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/24" xr:uid="{61814D74-0D5A-4E7E-AF68-2BC4F861AC78}"/>
     <hyperlink ref="F64:F67" r:id="rId7" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/24" xr:uid="{41855F6C-EE4E-4685-B895-714E487E64AF}"/>
     <hyperlink ref="F68" r:id="rId8" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/25" xr:uid="{0850A534-0490-40E6-8522-76C33F4DA16B}"/>
+    <hyperlink ref="F69" r:id="rId9" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/21" xr:uid="{C7A6AED9-4CEA-4F83-B009-A0E8FAF1B59E}"/>
+    <hyperlink ref="F70:F74" r:id="rId10" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/21" xr:uid="{E44CD4A0-8F59-442A-AF9F-81DFA6B012B8}"/>
+    <hyperlink ref="F77" r:id="rId11" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{2D468D44-CC33-4397-B10D-6A8CC1F5509F}"/>
+    <hyperlink ref="F78:F87" r:id="rId12" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{99F47488-7EFB-4D78-842D-BA8B8258C4A8}"/>
+    <hyperlink ref="F88:F98" r:id="rId13" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{9D2670DC-365B-4841-BD4F-11E66B03A343}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId14"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2208f11-ae8c-46f3-b7de-f72e1c6d0934">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC745917B956084FBC19C2B85F94DD54" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="865a07db5559135b02b49b365e0b81ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2208f11-ae8c-46f3-b7de-f72e1c6d0934" xmlns:ns3="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e91ff7f3783b5129c9128fce1d9ba9c" ns2:_="" ns3:_="">
     <xsd:import namespace="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
@@ -2463,14 +4130,66 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2208f11-ae8c-46f3-b7de-f72e1c6d0934">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D3F574-1D4C-41FF-8CB3-6F4DD5AF995B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F5A1BD-A9B3-477A-AFD5-C929335163D7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
+    <ds:schemaRef ds:uri="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3D8B3A-6998-4DF6-A0B6-219B9EFDF5AB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3D8B3A-6998-4DF6-A0B6-219B9EFDF5AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F5A1BD-A9B3-477A-AFD5-C929335163D7}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D3F574-1D4C-41FF-8CB3-6F4DD5AF995B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added Suite 008 test cases
</commit_message>
<xml_diff>
--- a/CDR Test Documentation CHANGE LOG.xlsx
+++ b/CDR Test Documentation CHANGE LOG.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_codeRepos\codeDataStandards\standards-testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://govteams.sharepoint.com/sites/datastandardsbody/Shared Documents/Standards and Guidelines/Testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A7A8B01-7D54-4AB3-86F8-727E4C179DE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="361" documentId="8_{9B3D86EA-31BB-4D21-B7B8-766CEFF32DB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38FA94F8-7BC9-42A6-B10E-D978C61C3908}"/>
   <bookViews>
-    <workbookView xWindow="-30828" yWindow="2256" windowWidth="30936" windowHeight="16896" xr2:uid="{E1E61262-89E5-4C9F-B6BD-CA910CFEB013}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E1E61262-89E5-4C9F-B6BD-CA910CFEB013}"/>
   </bookViews>
   <sheets>
     <sheet name="Change log" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="240">
   <si>
     <t>Change date</t>
   </si>
@@ -912,12 +912,45 @@
   <si>
     <t>Corrected various spellings of 'Response' and typos on 'Interaction', 'Version', 'i.e.', 'formatted' and 'correctly' throughout.</t>
   </si>
+  <si>
+    <t>1.0.3</t>
+  </si>
+  <si>
+    <t>T.EAR.008</t>
+  </si>
+  <si>
+    <t>PreCondition</t>
+  </si>
+  <si>
+    <t>Added 'invalid' to incomplete sentence and removed &lt;&gt; from servicePointId</t>
+  </si>
+  <si>
+    <t>A.EAA.001-006</t>
+  </si>
+  <si>
+    <t>Added Suite.008 Test Cases</t>
+  </si>
+  <si>
+    <t>Added Suite.008 Assertions</t>
+  </si>
+  <si>
+    <t>S.EAA.047-054</t>
+  </si>
+  <si>
+    <t>Test Cases</t>
+  </si>
+  <si>
+    <t>Added Test Case references to Scenarios</t>
+  </si>
+  <si>
+    <t>T.EAA.001-056</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -962,6 +995,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -990,7 +1029,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1018,6 +1057,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1334,27 +1376,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C4B9470-3BCE-4ABB-997A-921DA99601C0}">
-  <dimension ref="A1:F131"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C125" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C123" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K92" sqref="K92"/>
+      <selection pane="bottomRight" activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.109375" style="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="110.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="110.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.28515625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1374,7 +1416,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="8">
         <v>44700</v>
       </c>
@@ -1394,7 +1436,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>44715</v>
       </c>
@@ -1414,7 +1456,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="8">
         <v>44715</v>
       </c>
@@ -1434,7 +1476,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>44715</v>
       </c>
@@ -1454,7 +1496,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>44715</v>
       </c>
@@ -1474,7 +1516,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>44715</v>
       </c>
@@ -1494,7 +1536,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="8">
         <v>44715</v>
       </c>
@@ -1514,7 +1556,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>44715</v>
       </c>
@@ -1534,7 +1576,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="8">
         <v>44715</v>
       </c>
@@ -1554,7 +1596,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>44715</v>
       </c>
@@ -1574,7 +1616,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>44715</v>
       </c>
@@ -1594,7 +1636,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>44715</v>
       </c>
@@ -1614,7 +1656,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>44715</v>
       </c>
@@ -1634,7 +1676,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>44715</v>
       </c>
@@ -1654,7 +1696,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>44715</v>
       </c>
@@ -1674,7 +1716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>44715</v>
       </c>
@@ -1694,7 +1736,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>44715</v>
       </c>
@@ -1714,7 +1756,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>44715</v>
       </c>
@@ -1734,7 +1776,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>44715</v>
       </c>
@@ -1754,7 +1796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>44715</v>
       </c>
@@ -1774,7 +1816,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>44715</v>
       </c>
@@ -1794,7 +1836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
         <v>44715</v>
       </c>
@@ -1814,7 +1856,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
         <v>44715</v>
       </c>
@@ -1834,7 +1876,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
         <v>44715</v>
       </c>
@@ -1854,7 +1896,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>44715</v>
       </c>
@@ -1874,7 +1916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>44715</v>
       </c>
@@ -1894,7 +1936,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>44715</v>
       </c>
@@ -1914,7 +1956,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
         <v>44715</v>
       </c>
@@ -1934,7 +1976,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
         <v>44715</v>
       </c>
@@ -1954,7 +1996,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="8">
         <v>44715</v>
       </c>
@@ -1974,7 +2016,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="8">
         <v>44715</v>
       </c>
@@ -1994,7 +2036,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="8">
         <v>44715</v>
       </c>
@@ -2014,7 +2056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="8">
         <v>44715</v>
       </c>
@@ -2034,7 +2076,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="8">
         <v>44715</v>
       </c>
@@ -2054,7 +2096,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="8">
         <v>44715</v>
       </c>
@@ -2074,7 +2116,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="8">
         <v>44715</v>
       </c>
@@ -2094,7 +2136,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="8">
         <v>44715</v>
       </c>
@@ -2114,7 +2156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="8">
         <v>44715</v>
       </c>
@@ -2134,7 +2176,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="8">
         <v>44715</v>
       </c>
@@ -2154,7 +2196,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="8">
         <v>44715</v>
       </c>
@@ -2174,7 +2216,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="8">
         <v>44715</v>
       </c>
@@ -2194,7 +2236,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="8">
         <v>44715</v>
       </c>
@@ -2214,7 +2256,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="8">
         <v>44715</v>
       </c>
@@ -2234,7 +2276,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="8">
         <v>44715</v>
       </c>
@@ -2254,7 +2296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="8">
         <v>44715</v>
       </c>
@@ -2274,7 +2316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="8">
         <v>44715</v>
       </c>
@@ -2294,7 +2336,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="8">
         <v>44715</v>
       </c>
@@ -2314,7 +2356,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="8">
         <v>44715</v>
       </c>
@@ -2334,7 +2376,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="8">
         <v>44715</v>
       </c>
@@ -2354,7 +2396,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="8">
         <v>44715</v>
       </c>
@@ -2374,7 +2416,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="8">
         <v>44715</v>
       </c>
@@ -2394,7 +2436,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="8">
         <v>44715</v>
       </c>
@@ -2414,7 +2456,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="8">
         <v>44715</v>
       </c>
@@ -2434,7 +2476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="8">
         <v>44715</v>
       </c>
@@ -2454,7 +2496,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="8">
         <v>44715</v>
       </c>
@@ -2474,7 +2516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="8">
         <v>44715</v>
       </c>
@@ -2494,7 +2536,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="8">
         <v>44715</v>
       </c>
@@ -2514,7 +2556,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="8">
         <v>44715</v>
       </c>
@@ -2534,7 +2576,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="8">
         <v>44715</v>
       </c>
@@ -2554,7 +2596,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="8">
         <v>44715</v>
       </c>
@@ -2574,7 +2616,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="8">
         <v>44715</v>
       </c>
@@ -2594,7 +2636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="8">
         <v>44719</v>
       </c>
@@ -2614,7 +2656,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="8">
         <v>44719</v>
       </c>
@@ -2634,7 +2676,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="8">
         <v>44719</v>
       </c>
@@ -2654,7 +2696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="8">
         <v>44719</v>
       </c>
@@ -2674,7 +2716,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="8">
         <v>44719</v>
       </c>
@@ -2694,7 +2736,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="8">
         <v>44719</v>
       </c>
@@ -2714,7 +2756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="8">
         <v>44754</v>
       </c>
@@ -2734,7 +2776,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="8">
         <v>44754</v>
       </c>
@@ -2754,7 +2796,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="8">
         <v>44754</v>
       </c>
@@ -2774,7 +2816,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="8">
         <v>44754</v>
       </c>
@@ -2794,7 +2836,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="8">
         <v>44754</v>
       </c>
@@ -2814,7 +2856,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" s="8">
         <v>44754</v>
       </c>
@@ -2834,7 +2876,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" s="8">
         <v>44754</v>
       </c>
@@ -2852,7 +2894,7 @@
       </c>
       <c r="F75" s="4"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" s="8">
         <v>44754</v>
       </c>
@@ -2870,7 +2912,7 @@
       </c>
       <c r="F76" s="4"/>
     </row>
-    <row r="77" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A77" s="8">
         <v>44754</v>
       </c>
@@ -2890,7 +2932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A78" s="8">
         <v>44754</v>
       </c>
@@ -2910,7 +2952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A79" s="8">
         <v>44754</v>
       </c>
@@ -2930,7 +2972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="8">
         <v>44754</v>
       </c>
@@ -2950,7 +2992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A81" s="8">
         <v>44754</v>
       </c>
@@ -2970,7 +3012,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="8">
         <v>44754</v>
       </c>
@@ -2990,7 +3032,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="83" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A83" s="8">
         <v>44754</v>
       </c>
@@ -3010,7 +3052,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="84" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A84" s="8">
         <v>44754</v>
       </c>
@@ -3030,7 +3072,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A85" s="8">
         <v>44754</v>
       </c>
@@ -3050,7 +3092,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A86" s="8">
         <v>44754</v>
       </c>
@@ -3070,7 +3112,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A87" s="8">
         <v>44754</v>
       </c>
@@ -3090,7 +3132,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="88" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A88" s="8">
         <v>44754</v>
       </c>
@@ -3110,7 +3152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="89" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A89" s="8">
         <v>44754</v>
       </c>
@@ -3130,7 +3172,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="90" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A90" s="8">
         <v>44754</v>
       </c>
@@ -3150,7 +3192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="91" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A91" s="8">
         <v>44754</v>
       </c>
@@ -3170,7 +3212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="92" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A92" s="8">
         <v>44754</v>
       </c>
@@ -3190,7 +3232,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="93" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A93" s="8">
         <v>44754</v>
       </c>
@@ -3210,7 +3252,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A94" s="8">
         <v>44754</v>
       </c>
@@ -3230,7 +3272,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A95" s="8">
         <v>44754</v>
       </c>
@@ -3250,7 +3292,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="8">
         <v>44754</v>
       </c>
@@ -3270,7 +3312,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="8">
         <v>44754</v>
       </c>
@@ -3290,7 +3332,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A98" s="8">
         <v>44754</v>
       </c>
@@ -3310,7 +3352,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A99" s="8">
         <v>44754</v>
       </c>
@@ -3330,7 +3372,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A100" s="8">
         <v>44754</v>
       </c>
@@ -3350,7 +3392,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="101" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A101" s="8">
         <v>44754</v>
       </c>
@@ -3370,7 +3412,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="102" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A102" s="8">
         <v>44754</v>
       </c>
@@ -3390,7 +3432,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="103" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A103" s="8">
         <v>44754</v>
       </c>
@@ -3410,7 +3452,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="104" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A104" s="8">
         <v>44754</v>
       </c>
@@ -3430,7 +3472,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="105" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A105" s="8">
         <v>44754</v>
       </c>
@@ -3450,7 +3492,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="106" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A106" s="8">
         <v>44754</v>
       </c>
@@ -3470,7 +3512,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A107" s="8">
         <v>44754</v>
       </c>
@@ -3490,7 +3532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A108" s="8">
         <v>44754</v>
       </c>
@@ -3510,7 +3552,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A109" s="8">
         <v>44754</v>
       </c>
@@ -3530,7 +3572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A110" s="8">
         <v>44754</v>
       </c>
@@ -3550,7 +3592,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A111" s="8">
         <v>44754</v>
       </c>
@@ -3570,7 +3612,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A112" s="8">
         <v>44754</v>
       </c>
@@ -3590,7 +3632,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="180" x14ac:dyDescent="0.25">
       <c r="A113" s="8">
         <v>44754</v>
       </c>
@@ -3610,7 +3652,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A114" s="8">
         <v>44754</v>
       </c>
@@ -3630,7 +3672,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A115" s="8">
         <v>44754</v>
       </c>
@@ -3650,7 +3692,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A116" s="8">
         <v>44754</v>
       </c>
@@ -3670,7 +3712,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="135" x14ac:dyDescent="0.25">
       <c r="A117" s="8">
         <v>44754</v>
       </c>
@@ -3690,7 +3732,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A118" s="8">
         <v>44754</v>
       </c>
@@ -3710,7 +3752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="8">
         <v>44754</v>
       </c>
@@ -3730,7 +3772,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A120" s="8">
         <v>44754</v>
       </c>
@@ -3750,7 +3792,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A121" s="8">
         <v>44754</v>
       </c>
@@ -3770,7 +3812,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A122" s="8">
         <v>44754</v>
       </c>
@@ -3790,7 +3832,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A123" s="8">
         <v>44754</v>
       </c>
@@ -3810,7 +3852,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A124" s="8">
         <v>44754</v>
       </c>
@@ -3830,7 +3872,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="125" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A125" s="8">
         <v>44754</v>
       </c>
@@ -3850,7 +3892,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A126" s="8">
         <v>44754</v>
       </c>
@@ -3870,7 +3912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="127" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A127" s="8">
         <v>44754</v>
       </c>
@@ -3890,7 +3932,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="128" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A128" s="8">
         <v>44754</v>
       </c>
@@ -3910,7 +3952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="129" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A129" s="8">
         <v>44754</v>
       </c>
@@ -3930,7 +3972,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="130" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A130" s="8">
         <v>44754</v>
       </c>
@@ -3950,7 +3992,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A131" s="8">
         <v>44754</v>
       </c>
@@ -3968,6 +4010,86 @@
       </c>
       <c r="F131" s="1" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" s="8">
+        <v>44777</v>
+      </c>
+      <c r="B132" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="F132" s="4">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A133" s="8">
+        <v>44778</v>
+      </c>
+      <c r="B133" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="F133" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A134" s="8">
+        <v>44778</v>
+      </c>
+      <c r="B134" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="F134" s="4">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A135" s="8">
+        <v>44778</v>
+      </c>
+      <c r="B135" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F135" s="4">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -3987,33 +4109,16 @@
     <hyperlink ref="F78:F87" r:id="rId12" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{99F47488-7EFB-4D78-842D-BA8B8258C4A8}"/>
     <hyperlink ref="F88:F98" r:id="rId13" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{9D2670DC-365B-4841-BD4F-11E66B03A343}"/>
     <hyperlink ref="F99:F130" r:id="rId14" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/26" xr:uid="{BCF8CED7-A426-4CD2-A78B-CED48AC0A46C}"/>
+    <hyperlink ref="F132" r:id="rId15" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/38" xr:uid="{F404522D-925C-4222-AAEC-0A89159152D1}"/>
+    <hyperlink ref="F133" r:id="rId16" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/33" xr:uid="{C84F176F-83C4-4CF9-A3FB-1A6C6D08850F}"/>
+    <hyperlink ref="F134:F135" r:id="rId17" display="https://github.com/ConsumerDataStandardsAustralia/standards-testing/issues/33" xr:uid="{31FEE580-D060-4F03-9029-CC8301545EBE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId15"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2208f11-ae8c-46f3-b7de-f72e1c6d0934">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AC745917B956084FBC19C2B85F94DD54" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="865a07db5559135b02b49b365e0b81ea">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b2208f11-ae8c-46f3-b7de-f72e1c6d0934" xmlns:ns3="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5e91ff7f3783b5129c9128fce1d9ba9c" ns2:_="" ns3:_="">
     <xsd:import namespace="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
@@ -4250,32 +4355,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D3F574-1D4C-41FF-8CB3-6F4DD5AF995B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="b2208f11-ae8c-46f3-b7de-f72e1c6d0934">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3D8B3A-6998-4DF6-A0B6-219B9EFDF5AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5F5A1BD-A9B3-477A-AFD5-C929335163D7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4292,4 +4392,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F3D8B3A-6998-4DF6-A0B6-219B9EFDF5AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="b2208f11-ae8c-46f3-b7de-f72e1c6d0934"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f4f5ba83-536b-4bb3-a2e0-84bf902bc80d"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{86D3F574-1D4C-41FF-8CB3-6F4DD5AF995B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>